<commit_message>
Update on some files
</commit_message>
<xml_diff>
--- a/Password Times.xlsx
+++ b/Password Times.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{55A86C38-720D-4233-87A9-9EC7E89874DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B14F698E-2CF9-4CEE-8E01-8946132644B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="225" zoomScaleNormal="225" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -570,6 +570,9 @@
       <c r="B2" s="5">
         <v>806.45963300000005</v>
       </c>
+      <c r="C2">
+        <v>5214</v>
+      </c>
       <c r="D2" s="5">
         <v>27936.439836000001</v>
       </c>
@@ -684,9 +687,9 @@
         <f>AVERAGE(B2:B11)</f>
         <v>804.09822387000008</v>
       </c>
-      <c r="C12" s="14" t="e">
+      <c r="C12" s="14">
         <f>AVERAGE(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>5214</v>
       </c>
       <c r="D12" s="13">
         <f>AVERAGE(D2:D11)</f>

</xml_diff>